<commit_message>
fix filter WS and WK adreses
</commit_message>
<xml_diff>
--- a/topy.xlsx
+++ b/topy.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -427,387 +427,195 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>45178140</v>
+        <v>43183154</v>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">LOFT COTTAGE PEPPER V-SHAPE 300X320/50X9
-5901779370675
+          <t xml:space="preserve">PODŁ/D 038 ALFA YET 5CM 12PŁ 6M2
+5902578300740
 </t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">01R0628A
-01R0628B
-01R0627C40
-01R0822B10
-01R0624A60
+          <t xml:space="preserve">W0475 - 19
+W0470
+W0468
+W0476
 </t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>45360686</v>
+        <v>44655072</v>
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">TIKKURILA ANTI-REFLEX 10L WHITE
-6408070068618
+          <t xml:space="preserve">FASADA 040 STB 15CM 4PL 2M2
+5901845540322
 </t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">01R0129B30
-01R0129C30
-01R0123C10
-01R1014C20
-01R1431A20
-01R1205D30
-01R0932C40
-01R0326A20
-01R0932B20
+          <t xml:space="preserve">W0475 - 58
+W0466
+W0468
+W0474
+W0471
+W0470
 </t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>45460324</v>
+        <v>44956331</v>
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">ZESTAW SZAFKA Z/UM/LUST POINT 60 BIALY
-5906365473983
-5906365510404
-5906365406486
+          <t xml:space="preserve">ŁĄCZNIK PRZELOTOWY H 22X16 5X20 JON
+5901874920614
 </t>
         </is>
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">01R1422B30
-01R1433C20
-01R1433D30
-01R1431A40
-01R1425B40
-01R1433D40
-01R1025D20
-01R1005A20
-01R1205B10
-01R1211B10
-01R1405C10
-01R1317D20
-01R1409C20
-01R1401D10
-01R1403C20
-01R1401B30
-01R1326B30
-01R1124C10
-01R1008A30
-01R1009B30
-01R1027B30
-01R1321B20
-01R1321C10
-01R1321C30
-01R1309D10
-01R0825C50
-01R0620B30
-01R0621C20
-01R0624B30
-01R1024B10
-01R0533D10
-01R0621A60
-01R0621B60
-01R1231D30
-01R1229D10
-01R0821D20
-01R0617A2
-01R1014B20
-01R0617B10
-01R0617A40
-01R0524D20
-01R0532D30
-01R0822C10
-01R1310C20
-01R1122C10
-01R1133A20
-01R1005B10
-01R0319C40
-01R1203B40
-01R0317C40
-01R0820B30
-01R0831A70
+          <t xml:space="preserve">W0116 - 28
+W0114 - 259
+W0115 - 52
+W0122 - 59
+W0336
 </t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>45503843</v>
+        <v>45244584</v>
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">LISTWA SV-15 J-TRIM GRAFIT 3 05M
-5905952159989
+          <t xml:space="preserve">BAT WANN SENSEA INARI CHR Z/ZEST
+5901171185044
 </t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">W0270
-01M522-10
-01M504-30
-01M507-10
-01M533-10
-01M504-10
-01M122-20
-01M514-10
-01M208
-01M217
-01M117-20
-01M116-20
-01M216
-01M106-10
-01M124-20
-01M117-10
-01M126-10
+          <t xml:space="preserve">K0800301 - 1
+01R0726B20 - 1
+K1504906
+K1504302
+01R0534B40
+K0007903
+K0502401
+K0501201
+01R0517A50
+01R0833C30
 </t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>45587696</v>
+        <v>45682616</v>
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">NAR ZEW ESQUERO 609 SOSNA ZWYCZAJNA
-2000455876961
-5905952183366
+          <t xml:space="preserve">.KORA DROBNA PODKŁADOWA 50L SOB
+5908235396415
 </t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">K0813901
-01R1015D20
-K0301206
+          <t xml:space="preserve">W0463 - 1
 </t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>45750054</v>
+        <v>82662005</v>
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">ZASLEPKA SAMO 20MM CZARNY 12SZT
-5901912822849
+          <t xml:space="preserve">MOZ 28.8X29.25 METRO GREEN  GLOSSY
+3276007151398
 </t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">K1300411
-K1501509
-K0502704
-K0904407
+          <t xml:space="preserve">01R0721C60 - 5
+01R0817D40
+01R0817D40
+01R0830B10
+01R0830C10
 </t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>45810940</v>
+        <v>82680051</v>
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">LAMPA STOJ NEW YORK 44+GN 12W E27 GRAFIT
-5901508307323
+          <t xml:space="preserve">GL 30X90 LARCHWOOD ALDER 1 08/4
+2000826800511
+8433019220992
 </t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">01R0829B10
-01R1209A30
-01R0326C10
-K1705301
-01R1014C20
-K0505402
-01R1014C10
-01R1014D10
-01R0833C40
-01R0833D40
-01R0833A50
-01R0617D50
-01R0729D20
-01R1008B40
-01R0328A10
-01R1404D10
-01R0834A60
-01R1232B10
-01R1232A10
-01R1404C10
+          <t xml:space="preserve">01R0920C50 - 2
+01R0633B50
+01R0621C10
+01R0818D
+01R0222D30
+01R0620C30
+01R0723D10
+02R0141D40
+01R0930C20
+01R0723D60
+01R0822A30
+01R0531A70
+01R0522B
+01R0820C50
+01R0817B30
+01R0127C10
+01R0934B30
+01R0828A50
+01R0623A10
+01R0622B50
+01R0820D50
+01R0334B50
+01R0930B30
 </t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>45887233</v>
+        <v>89180504</v>
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">LACZNIK 56 411 KLASYCZNA 2SZT
-5902537595774
-5902537596085
+          <t xml:space="preserve">KLIN SPRĘŻYNOWY DO MONTAŻU PARAPETU 5SZT
+5907796632406
 </t>
         </is>
       </c>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">K0713803
-K1301708
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>82135692</v>
-      </c>
-      <c r="B9" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">QUADRO 45 RAMKA 2X CZARNY KW
-5603011623807
-2000821356921
-</t>
-        </is>
-      </c>
-      <c r="C9" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">K0500205
-K0811501
-K1104804
-K1305707
-K1300207
-K0303303
-K0004104
-K1702207
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>82406231</v>
-      </c>
-      <c r="B10" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">OPASKA NIERDZ TAŚMOWA 8-15MM 2SZT RIM
-5905620028647
-2000824062311
-</t>
-        </is>
-      </c>
-      <c r="C10" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">K1301609
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>82798140</v>
-      </c>
-      <c r="B11" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">DEXTER PEDZEL PLASKI CR ROZP 30MM
-2000827981401
-3276007190625
-</t>
-        </is>
-      </c>
-      <c r="C11" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">K1300705
-K0607604
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>83023651</v>
-      </c>
-      <c r="B12" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CURVER POJEMNIK LUNCH KIT ZIELONY 1 2L
-3253920947000
-</t>
-        </is>
-      </c>
-      <c r="C12" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">K1219702
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>83280642</v>
-      </c>
-      <c r="B13" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">GL 39 8X119 8 COFFEE FOAM WHITE 0 95/2
-5902115791345
-</t>
-        </is>
-      </c>
-      <c r="C13" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">01R0822D30
-01R0720A30
-01R0629C
-01R0825A30
-01R0727A40
-01R0922D20
-01R0729C20
-01R0819D20
-01R0621A30
-01R0818A60
-01R0822B
-01R0930C20
-01R0117D20
-01R0832C50
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>916403</v>
-      </c>
-      <c r="B14" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ZESTAW 4 HACZYKOW STAL SZCZOT
-20009164031
-3276000368236
-</t>
-        </is>
-      </c>
-      <c r="C14" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">K1300701
-K1300709
-K0000903
+          <t xml:space="preserve">01R1313C10 - 21
+01R1313B20
+01R1313A20
+K0912105
 </t>
         </is>
       </c>

</xml_diff>